<commit_message>
redid something I have no clue
</commit_message>
<xml_diff>
--- a/Sternberg_2/conditions.xlsx
+++ b/Sternberg_2/conditions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\04Ben\OneDrive\Desktop\Sternberg_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\04Ben\github\mstembci\Sternberg_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5B4A52-C1B3-43E6-896B-89520C2EB028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F7A25B-19BB-4645-8C1E-E1149942D2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="1280" windowWidth="12830" windowHeight="11710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>cross_time</t>
   </si>
@@ -37,15 +37,6 @@
   </si>
   <si>
     <t>feedback_time</t>
-  </si>
-  <si>
-    <t>key_resp</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>.</t>
   </si>
   <si>
     <t>response_time</t>
@@ -372,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -389,7 +380,7 @@
     <col min="7" max="7" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,19 +394,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -436,14 +424,6 @@
       </c>
       <c r="G2">
         <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>